<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => brominated
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/brominated/summarised_levels_data_brominated_ww.xlsx
+++ b/inst/results/data_contam/brominated/summarised_levels_data_brominated_ww.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,12 +375,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>median_1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median_2</t>
+          <t>median_percent</t>
         </is>
       </c>
     </row>
@@ -396,13 +391,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>0.01275</v>
       </c>
       <c r="D2">
-        <v>0.02186</v>
-      </c>
-      <c r="E2">
-        <v>0.005988</v>
+        <v>0.007634730538922156</v>
       </c>
     </row>
     <row r="3">
@@ -417,13 +409,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.014</v>
+        <v>0.0255</v>
       </c>
       <c r="D3">
-        <v>0.02404</v>
-      </c>
-      <c r="E3">
-        <v>0.008383</v>
+        <v>0.01526946107784431</v>
       </c>
     </row>
     <row r="4">
@@ -438,13 +427,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.089</v>
+        <v>0.138</v>
       </c>
       <c r="D4">
-        <v>0.1767</v>
-      </c>
-      <c r="E4">
-        <v>0.05329</v>
+        <v>0.08263473053892217</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +445,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.0007</v>
+        <v>0.00035</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.0004192</v>
+        <v>0.0002095808383233533</v>
       </c>
     </row>
     <row r="6">
@@ -480,14 +463,11 @@
         </is>
       </c>
       <c r="C6">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0.0005988</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -501,13 +481,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="D7">
-        <v>0.006587</v>
-      </c>
-      <c r="E7">
-        <v>0.007186</v>
+        <v>0.00658682634730539</v>
       </c>
     </row>
     <row r="8">
@@ -525,10 +502,7 @@
         <v>0.002</v>
       </c>
       <c r="D8">
-        <v>0.001198</v>
-      </c>
-      <c r="E8">
-        <v>0.001198</v>
+        <v>0.001197604790419162</v>
       </c>
     </row>
     <row r="9">
@@ -543,13 +517,10 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D9">
-        <v>0.002994</v>
-      </c>
-      <c r="E9">
-        <v>0.001198</v>
+        <v>0.001796407185628743</v>
       </c>
     </row>
     <row r="10">
@@ -564,13 +535,10 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.106</v>
+        <v>0.091</v>
       </c>
       <c r="D10">
-        <v>0.05449</v>
-      </c>
-      <c r="E10">
-        <v>0.06347</v>
+        <v>0.05449101796407185</v>
       </c>
     </row>
     <row r="11">
@@ -585,13 +553,10 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.0371</v>
+        <v>0.077</v>
       </c>
       <c r="D11">
-        <v>2405</v>
-      </c>
-      <c r="E11">
-        <v>436.5</v>
+        <v>905.8823529411765</v>
       </c>
     </row>
     <row r="12">
@@ -606,13 +571,10 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.0444</v>
+        <v>0.08995</v>
       </c>
       <c r="D12">
-        <v>1924</v>
-      </c>
-      <c r="E12">
-        <v>522.4</v>
+        <v>1058.235294117647</v>
       </c>
     </row>
     <row r="13">
@@ -627,13 +589,10 @@
         </is>
       </c>
       <c r="C13">
-        <v>0.148</v>
+        <v>0.33185</v>
       </c>
       <c r="D13">
-        <v>7212</v>
-      </c>
-      <c r="E13">
-        <v>1741</v>
+        <v>3904.117647058823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>